<commit_message>
Add analysis parameter variables
</commit_message>
<xml_diff>
--- a/biokapacitas_okologiai_labnyom_2Bnelkul_neparannyal.xlsx
+++ b/biokapacitas_okologiai_labnyom_2Bnelkul_neparannyal.xlsx
@@ -1,27 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Peter\Desktop\ecological_footprint_clustering\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20538295-FBB2-4626-BC3D-72EF1F46B17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16452" windowHeight="5832" activeTab="1"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka3" sheetId="3" r:id="rId1"/>
     <sheet name="Munka1" sheetId="4" r:id="rId2"/>
     <sheet name="Munka2" sheetId="5" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="561">
   <si>
     <t>Ország</t>
   </si>
@@ -1601,18 +1616,9 @@
     <t>Szlovénia</t>
   </si>
   <si>
-    <t>Nitnegra</t>
-  </si>
-  <si>
     <t>Ireza</t>
   </si>
   <si>
-    <t>Sedalgnab</t>
-  </si>
-  <si>
-    <t>Anawstob</t>
-  </si>
-  <si>
     <t>Idnurub</t>
   </si>
   <si>
@@ -1676,9 +1682,6 @@
     <t>Adnaur</t>
   </si>
   <si>
-    <t>Bára-Duasz</t>
-  </si>
-  <si>
     <t>Sinut</t>
   </si>
   <si>
@@ -1691,14 +1694,38 @@
     <t>Initawse</t>
   </si>
   <si>
-    <t>Nevols</t>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Shedalgnab</t>
+  </si>
+  <si>
+    <t>Hajidúasz-Sza</t>
+  </si>
+  <si>
+    <t>Szomália</t>
+  </si>
+  <si>
+    <t>Ayilaamoos</t>
+  </si>
+  <si>
+    <t>Yaugarap</t>
+  </si>
+  <si>
+    <t>Paraguay</t>
+  </si>
+  <si>
+    <t>Elich</t>
+  </si>
+  <si>
+    <t>Chile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1715,6 +1742,12 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1754,7 +1787,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1775,6 +1808,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -1797,30 +1831,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Táblázat2" displayName="Táblázat2" ref="A1:R1048530" totalsRowShown="0">
-  <autoFilter ref="A1:R1048530"/>
-  <sortState ref="A2:R321">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Táblázat2" displayName="Táblázat2" ref="A1:R1048530" totalsRowShown="0">
+  <autoFilter ref="A1:R1048530" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R321">
     <sortCondition descending="1" ref="K2"/>
   </sortState>
   <tableColumns count="18">
-    <tableColumn id="1" name="Ország"/>
-    <tableColumn id="2" name="Épített"/>
-    <tableColumn id="3" name="Karbon"/>
-    <tableColumn id="4" name="Szántó"/>
-    <tableColumn id="5" name="Hal"/>
-    <tableColumn id="6" name="Erdő"/>
-    <tableColumn id="7" name="Legelő"/>
-    <tableColumn id="8" name="Összes"/>
-    <tableColumn id="9" name="Összes a táblázatban"/>
-    <tableColumn id="10" name="Adatminőség" dataDxfId="0"/>
-    <tableColumn id="11" name="Államalkotó népesség aránya"/>
-    <tableColumn id="12" name="Oszlop2"/>
-    <tableColumn id="13" name="Oszlop3"/>
-    <tableColumn id="14" name="Oszlop4"/>
-    <tableColumn id="15" name="Oszlop5"/>
-    <tableColumn id="16" name="Oszlop6"/>
-    <tableColumn id="17" name="Oszlop7"/>
-    <tableColumn id="18" name="Oszlop8"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ország"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Épített"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Karbon"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Szántó"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Hal"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Erdő"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Legelő"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Összes"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Összes a táblázatban"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Adatminőség" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Államalkotó népesség aránya"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Oszlop2"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Oszlop3"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Oszlop4"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Oszlop5"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Oszlop6"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Oszlop7"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="Oszlop8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2081,28 +2115,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R321"/>
   <sheetViews>
     <sheetView topLeftCell="A114" workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="24.44140625" customWidth="1"/>
+    <col min="1" max="1" width="27.53125" customWidth="1"/>
+    <col min="10" max="10" width="10.1328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="24.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2158,7 +2192,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>132</v>
       </c>
@@ -2193,7 +2227,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -2228,7 +2262,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2261,7 +2295,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>250</v>
       </c>
@@ -2296,7 +2330,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>340</v>
       </c>
@@ -2332,7 +2366,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>296</v>
       </c>
@@ -2367,7 +2401,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>255</v>
       </c>
@@ -2402,7 +2436,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>189</v>
       </c>
@@ -2437,7 +2471,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2472,7 +2506,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>310</v>
       </c>
@@ -2507,7 +2541,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>179</v>
       </c>
@@ -2542,7 +2576,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>61</v>
       </c>
@@ -2577,7 +2611,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -2612,7 +2646,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>89</v>
       </c>
@@ -2647,7 +2681,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -2682,7 +2716,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>294</v>
       </c>
@@ -2717,7 +2751,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -2753,7 +2787,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>240</v>
       </c>
@@ -2788,7 +2822,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>65</v>
       </c>
@@ -2823,7 +2857,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>266</v>
       </c>
@@ -2858,7 +2892,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>232</v>
       </c>
@@ -2893,7 +2927,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>325</v>
       </c>
@@ -2928,7 +2962,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>243</v>
       </c>
@@ -2963,7 +2997,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>114</v>
       </c>
@@ -2998,7 +3032,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>46</v>
       </c>
@@ -3033,7 +3067,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>197</v>
       </c>
@@ -3068,7 +3102,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>134</v>
       </c>
@@ -3103,7 +3137,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>286</v>
       </c>
@@ -3138,7 +3172,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>319</v>
       </c>
@@ -3174,7 +3208,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>312</v>
       </c>
@@ -3210,7 +3244,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>112</v>
       </c>
@@ -3245,7 +3279,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>276</v>
       </c>
@@ -3280,7 +3314,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -3316,7 +3350,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>163</v>
       </c>
@@ -3351,7 +3385,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>260</v>
       </c>
@@ -3386,7 +3420,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>173</v>
       </c>
@@ -3421,7 +3455,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>64</v>
       </c>
@@ -3456,7 +3490,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>116</v>
       </c>
@@ -3491,7 +3525,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>308</v>
       </c>
@@ -3526,7 +3560,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>375</v>
       </c>
@@ -3561,7 +3595,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>153</v>
       </c>
@@ -3596,7 +3630,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>300</v>
       </c>
@@ -3631,7 +3665,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>278</v>
       </c>
@@ -3666,7 +3700,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>304</v>
       </c>
@@ -3701,7 +3735,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>242</v>
       </c>
@@ -3736,7 +3770,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>56</v>
       </c>
@@ -3771,7 +3805,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -3806,7 +3840,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>24</v>
       </c>
@@ -3842,7 +3876,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>280</v>
       </c>
@@ -3877,7 +3911,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>270</v>
       </c>
@@ -3912,7 +3946,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>264</v>
       </c>
@@ -3947,7 +3981,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>79</v>
       </c>
@@ -3982,7 +4016,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>136</v>
       </c>
@@ -4017,7 +4051,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>370</v>
       </c>
@@ -4052,7 +4086,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>248</v>
       </c>
@@ -4087,7 +4121,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>22</v>
       </c>
@@ -4123,7 +4157,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>314</v>
       </c>
@@ -4159,7 +4193,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>28</v>
       </c>
@@ -4195,7 +4229,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>306</v>
       </c>
@@ -4230,7 +4264,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>289</v>
       </c>
@@ -4265,7 +4299,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>274</v>
       </c>
@@ -4300,7 +4334,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>292</v>
       </c>
@@ -4335,7 +4369,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>238</v>
       </c>
@@ -4370,7 +4404,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>209</v>
       </c>
@@ -4405,7 +4439,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>36</v>
       </c>
@@ -4441,7 +4475,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>302</v>
       </c>
@@ -4476,7 +4510,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>151</v>
       </c>
@@ -4511,7 +4545,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>262</v>
       </c>
@@ -4546,7 +4580,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>110</v>
       </c>
@@ -4581,7 +4615,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>298</v>
       </c>
@@ -4616,7 +4650,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>272</v>
       </c>
@@ -4651,7 +4685,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>155</v>
       </c>
@@ -4686,7 +4720,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>107</v>
       </c>
@@ -4721,7 +4755,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>195</v>
       </c>
@@ -4756,7 +4790,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>71</v>
       </c>
@@ -4791,7 +4825,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>34</v>
       </c>
@@ -4827,7 +4861,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>193</v>
       </c>
@@ -4862,7 +4896,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>215</v>
       </c>
@@ -4897,7 +4931,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>124</v>
       </c>
@@ -4932,7 +4966,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -4967,7 +5001,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -5002,7 +5036,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>199</v>
       </c>
@@ -5037,7 +5071,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>211</v>
       </c>
@@ -5072,7 +5106,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>329</v>
       </c>
@@ -5107,7 +5141,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>236</v>
       </c>
@@ -5142,7 +5176,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>284</v>
       </c>
@@ -5177,7 +5211,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>150</v>
       </c>
@@ -5212,7 +5246,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>128</v>
       </c>
@@ -5247,7 +5281,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>139</v>
       </c>
@@ -5282,7 +5316,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>118</v>
       </c>
@@ -5317,7 +5351,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>69</v>
       </c>
@@ -5352,7 +5386,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>220</v>
       </c>
@@ -5387,7 +5421,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>81</v>
       </c>
@@ -5422,7 +5456,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>39</v>
       </c>
@@ -5457,7 +5491,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>224</v>
       </c>
@@ -5492,7 +5526,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>143</v>
       </c>
@@ -5527,7 +5561,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>137</v>
       </c>
@@ -5562,7 +5596,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>126</v>
       </c>
@@ -5597,7 +5631,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>167</v>
       </c>
@@ -5632,7 +5666,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>130</v>
       </c>
@@ -5667,7 +5701,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>226</v>
       </c>
@@ -5702,7 +5736,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>105</v>
       </c>
@@ -5737,7 +5771,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>234</v>
       </c>
@@ -5772,7 +5806,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>73</v>
       </c>
@@ -5807,7 +5841,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>159</v>
       </c>
@@ -5842,7 +5876,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>145</v>
       </c>
@@ -5877,7 +5911,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>316</v>
       </c>
@@ -5912,7 +5946,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>161</v>
       </c>
@@ -5947,7 +5981,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>41</v>
       </c>
@@ -5982,7 +6016,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>44</v>
       </c>
@@ -6017,7 +6051,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>157</v>
       </c>
@@ -6052,7 +6086,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>327</v>
       </c>
@@ -6087,7 +6121,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>181</v>
       </c>
@@ -6122,7 +6156,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>268</v>
       </c>
@@ -6157,7 +6191,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>252</v>
       </c>
@@ -6192,7 +6226,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>321</v>
       </c>
@@ -6227,7 +6261,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>204</v>
       </c>
@@ -6262,7 +6296,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>20</v>
       </c>
@@ -6297,7 +6331,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>54</v>
       </c>
@@ -6332,7 +6366,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>85</v>
       </c>
@@ -6367,7 +6401,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>368</v>
       </c>
@@ -6402,7 +6436,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>93</v>
       </c>
@@ -6437,7 +6471,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>99</v>
       </c>
@@ -6472,7 +6506,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>103</v>
       </c>
@@ -6507,7 +6541,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>95</v>
       </c>
@@ -6542,7 +6576,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>203</v>
       </c>
@@ -6577,7 +6611,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>175</v>
       </c>
@@ -6612,7 +6646,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>83</v>
       </c>
@@ -6647,7 +6681,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>213</v>
       </c>
@@ -6682,7 +6716,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>75</v>
       </c>
@@ -6717,7 +6751,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>147</v>
       </c>
@@ -6752,7 +6786,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>222</v>
       </c>
@@ -6787,7 +6821,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>185</v>
       </c>
@@ -6822,7 +6856,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>60</v>
       </c>
@@ -6857,7 +6891,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>122</v>
       </c>
@@ -6892,7 +6926,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>191</v>
       </c>
@@ -6927,7 +6961,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>43</v>
       </c>
@@ -6962,7 +6996,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>169</v>
       </c>
@@ -6997,7 +7031,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>201</v>
       </c>
@@ -7032,7 +7066,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>182</v>
       </c>
@@ -7067,7 +7101,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>141</v>
       </c>
@@ -7102,7 +7136,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>187</v>
       </c>
@@ -7137,7 +7171,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>97</v>
       </c>
@@ -7172,7 +7206,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>230</v>
       </c>
@@ -7207,7 +7241,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>120</v>
       </c>
@@ -7242,7 +7276,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>258</v>
       </c>
@@ -7277,7 +7311,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>48</v>
       </c>
@@ -7312,7 +7346,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>245</v>
       </c>
@@ -7347,7 +7381,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>229</v>
       </c>
@@ -7382,7 +7416,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>207</v>
       </c>
@@ -7417,7 +7451,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>290</v>
       </c>
@@ -7452,7 +7486,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>323</v>
       </c>
@@ -7487,7 +7521,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>91</v>
       </c>
@@ -7522,7 +7556,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>101</v>
       </c>
@@ -7557,7 +7591,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>218</v>
       </c>
@@ -7592,7 +7626,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>165</v>
       </c>
@@ -7627,7 +7661,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>177</v>
       </c>
@@ -7662,7 +7696,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>282</v>
       </c>
@@ -7697,7 +7731,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>25</v>
       </c>
@@ -7733,7 +7767,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>384</v>
       </c>
@@ -7768,7 +7802,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>21</v>
       </c>
@@ -7801,7 +7835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>23</v>
       </c>
@@ -7834,7 +7868,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>217</v>
       </c>
@@ -7867,7 +7901,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>26</v>
       </c>
@@ -7900,7 +7934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>320</v>
       </c>
@@ -7933,7 +7967,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>29</v>
       </c>
@@ -7966,7 +8000,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>31</v>
       </c>
@@ -7999,7 +8033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>33</v>
       </c>
@@ -8032,7 +8066,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>313</v>
       </c>
@@ -8065,7 +8099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>35</v>
       </c>
@@ -8098,7 +8132,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>341</v>
       </c>
@@ -8131,7 +8165,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>37</v>
       </c>
@@ -8164,7 +8198,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>40</v>
       </c>
@@ -8196,7 +8230,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>42</v>
       </c>
@@ -8228,7 +8262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>317</v>
       </c>
@@ -8260,7 +8294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="177" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>318</v>
       </c>
@@ -8292,7 +8326,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="178" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>45</v>
       </c>
@@ -8324,7 +8358,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="179" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>47</v>
       </c>
@@ -8356,7 +8390,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="180" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>49</v>
       </c>
@@ -8388,7 +8422,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="181" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>51</v>
       </c>
@@ -8420,7 +8454,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="182" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>53</v>
       </c>
@@ -8452,7 +8486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="183" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>55</v>
       </c>
@@ -8484,7 +8518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="184" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>57</v>
       </c>
@@ -8516,7 +8550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="185" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>62</v>
       </c>
@@ -8548,7 +8582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>63</v>
       </c>
@@ -8580,7 +8614,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="187" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>59</v>
       </c>
@@ -8612,7 +8646,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="188" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>66</v>
       </c>
@@ -8644,7 +8678,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="189" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>68</v>
       </c>
@@ -8676,7 +8710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="190" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>188</v>
       </c>
@@ -8708,7 +8742,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="191" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>190</v>
       </c>
@@ -8740,7 +8774,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="192" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>192</v>
       </c>
@@ -8772,7 +8806,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="193" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>72</v>
       </c>
@@ -8804,7 +8838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="194" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>70</v>
       </c>
@@ -8836,7 +8870,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="195" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>371</v>
       </c>
@@ -8868,7 +8902,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="196" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>369</v>
       </c>
@@ -8900,7 +8934,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="197" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>305</v>
       </c>
@@ -8932,7 +8966,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="198" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>376</v>
       </c>
@@ -8964,7 +8998,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="199" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>231</v>
       </c>
@@ -8996,7 +9030,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="200" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>74</v>
       </c>
@@ -9028,7 +9062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="201" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>251</v>
       </c>
@@ -9060,7 +9094,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="202" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>237</v>
       </c>
@@ -9092,7 +9126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="203" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>76</v>
       </c>
@@ -9124,7 +9158,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="204" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>315</v>
       </c>
@@ -9157,7 +9191,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="205" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>385</v>
       </c>
@@ -9189,7 +9223,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="206" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>78</v>
       </c>
@@ -9221,7 +9255,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="207" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>82</v>
       </c>
@@ -9253,7 +9287,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="208" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>80</v>
       </c>
@@ -9285,7 +9319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="209" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>254</v>
       </c>
@@ -9317,7 +9351,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="210" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>84</v>
       </c>
@@ -9349,7 +9383,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="211" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>86</v>
       </c>
@@ -9381,7 +9415,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="212" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>322</v>
       </c>
@@ -9413,7 +9447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="213" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>90</v>
       </c>
@@ -9445,7 +9479,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="214" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>88</v>
       </c>
@@ -9477,7 +9511,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="215" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>92</v>
       </c>
@@ -9509,7 +9543,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="216" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>94</v>
       </c>
@@ -9541,7 +9575,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="217" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>96</v>
       </c>
@@ -9573,7 +9607,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="218" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>98</v>
       </c>
@@ -9605,7 +9639,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="219" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>100</v>
       </c>
@@ -9637,7 +9671,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="220" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>102</v>
       </c>
@@ -9669,7 +9703,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="221" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>164</v>
       </c>
@@ -9701,7 +9735,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="222" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>233</v>
       </c>
@@ -9733,7 +9767,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="223" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>104</v>
       </c>
@@ -9765,7 +9799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="224" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>324</v>
       </c>
@@ -9797,7 +9831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="225" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>108</v>
       </c>
@@ -9829,7 +9863,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="226" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>106</v>
       </c>
@@ -9861,7 +9895,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="227" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>109</v>
       </c>
@@ -9893,7 +9927,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="228" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>111</v>
       </c>
@@ -9925,7 +9959,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="229" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>113</v>
       </c>
@@ -9957,7 +9991,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="230" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>115</v>
       </c>
@@ -9989,7 +10023,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="231" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>311</v>
       </c>
@@ -10021,7 +10055,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="232" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>117</v>
       </c>
@@ -10053,7 +10087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="233" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>219</v>
       </c>
@@ -10085,7 +10119,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="234" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>221</v>
       </c>
@@ -10117,7 +10151,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="235" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>259</v>
       </c>
@@ -10149,7 +10183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="236" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>119</v>
       </c>
@@ -10181,7 +10215,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="237" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>295</v>
       </c>
@@ -10213,7 +10247,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="238" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>121</v>
       </c>
@@ -10245,7 +10279,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="239" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>326</v>
       </c>
@@ -10277,7 +10311,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="240" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>125</v>
       </c>
@@ -10309,7 +10343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>225</v>
       </c>
@@ -10341,7 +10375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>227</v>
       </c>
@@ -10373,7 +10407,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>228</v>
       </c>
@@ -10405,7 +10439,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>223</v>
       </c>
@@ -10437,7 +10471,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>235</v>
       </c>
@@ -10469,7 +10503,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>123</v>
       </c>
@@ -10501,7 +10535,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>127</v>
       </c>
@@ -10533,7 +10567,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>256</v>
       </c>
@@ -10565,7 +10599,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>133</v>
       </c>
@@ -10597,7 +10631,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>129</v>
       </c>
@@ -10629,7 +10663,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>131</v>
       </c>
@@ -10661,7 +10695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>246</v>
       </c>
@@ -10693,7 +10727,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>135</v>
       </c>
@@ -10725,7 +10759,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>247</v>
       </c>
@@ -10757,7 +10791,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>138</v>
       </c>
@@ -10789,7 +10823,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>140</v>
       </c>
@@ -10821,7 +10855,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>142</v>
       </c>
@@ -10853,7 +10887,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>241</v>
       </c>
@@ -10885,7 +10919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="259" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>146</v>
       </c>
@@ -10917,7 +10951,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>144</v>
       </c>
@@ -10949,7 +10983,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>148</v>
       </c>
@@ -10981,7 +11015,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>156</v>
       </c>
@@ -11013,7 +11047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>249</v>
       </c>
@@ -11045,7 +11079,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>149</v>
       </c>
@@ -11077,7 +11111,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>330</v>
       </c>
@@ -11109,7 +11143,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>152</v>
       </c>
@@ -11141,7 +11175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>154</v>
       </c>
@@ -11173,7 +11207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>328</v>
       </c>
@@ -11205,7 +11239,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>158</v>
       </c>
@@ -11237,7 +11271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>160</v>
       </c>
@@ -11269,7 +11303,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>239</v>
       </c>
@@ -11301,7 +11335,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>162</v>
       </c>
@@ -11333,7 +11367,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>166</v>
       </c>
@@ -11365,7 +11399,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>168</v>
       </c>
@@ -11397,7 +11431,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>170</v>
       </c>
@@ -11429,7 +11463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>172</v>
       </c>
@@ -11461,7 +11495,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>244</v>
       </c>
@@ -11493,7 +11527,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>174</v>
       </c>
@@ -11525,7 +11559,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="279" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>263</v>
       </c>
@@ -11557,7 +11591,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>27</v>
       </c>
@@ -11590,7 +11624,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>253</v>
       </c>
@@ -11622,7 +11656,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>176</v>
       </c>
@@ -11654,7 +11688,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>178</v>
       </c>
@@ -11686,7 +11720,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>180</v>
       </c>
@@ -11718,7 +11752,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>184</v>
       </c>
@@ -11750,7 +11784,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>257</v>
       </c>
@@ -11782,7 +11816,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>261</v>
       </c>
@@ -11814,7 +11848,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>265</v>
       </c>
@@ -11846,7 +11880,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>186</v>
       </c>
@@ -11878,7 +11912,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>194</v>
       </c>
@@ -11910,7 +11944,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>196</v>
       </c>
@@ -11942,7 +11976,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>198</v>
       </c>
@@ -11974,7 +12008,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>202</v>
       </c>
@@ -12006,7 +12040,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>285</v>
       </c>
@@ -12038,7 +12072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>283</v>
       </c>
@@ -12070,7 +12104,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>267</v>
       </c>
@@ -12102,7 +12136,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>269</v>
       </c>
@@ -12134,7 +12168,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>271</v>
       </c>
@@ -12166,7 +12200,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>273</v>
       </c>
@@ -12198,7 +12232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>287</v>
       </c>
@@ -12230,7 +12264,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>275</v>
       </c>
@@ -12262,7 +12296,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>277</v>
       </c>
@@ -12294,7 +12328,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>279</v>
       </c>
@@ -12326,7 +12360,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>200</v>
       </c>
@@ -12358,7 +12392,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>281</v>
       </c>
@@ -12390,7 +12424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>288</v>
       </c>
@@ -12422,7 +12456,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>291</v>
       </c>
@@ -12454,7 +12488,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>293</v>
       </c>
@@ -12486,7 +12520,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="309" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>205</v>
       </c>
@@ -12518,7 +12552,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A310" t="s">
         <v>299</v>
       </c>
@@ -12550,7 +12584,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A311" t="s">
         <v>206</v>
       </c>
@@ -12582,7 +12616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A312" t="s">
         <v>297</v>
       </c>
@@ -12614,7 +12648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A313" t="s">
         <v>301</v>
       </c>
@@ -12646,7 +12680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A314" t="s">
         <v>208</v>
       </c>
@@ -12678,7 +12712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="315" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A315" t="s">
         <v>303</v>
       </c>
@@ -12710,7 +12744,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A316" t="s">
         <v>210</v>
       </c>
@@ -12742,7 +12776,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="317" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A317" t="s">
         <v>307</v>
       </c>
@@ -12774,7 +12808,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A318" t="s">
         <v>212</v>
       </c>
@@ -12806,7 +12840,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A319" t="s">
         <v>309</v>
       </c>
@@ -12838,7 +12872,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A320" t="s">
         <v>214</v>
       </c>
@@ -12870,7 +12904,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A321" t="s">
         <v>216</v>
       </c>
@@ -12912,19 +12946,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -12959,7 +12993,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
         <v>496</v>
       </c>
@@ -12989,7 +13023,7 @@
         <v>6.84</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="6" t="s">
         <v>500</v>
       </c>
@@ -13025,7 +13059,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="6" t="s">
         <v>501</v>
       </c>
@@ -13061,7 +13095,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="6" t="s">
         <v>502</v>
       </c>
@@ -13096,7 +13130,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="6" t="s">
         <v>499</v>
       </c>
@@ -13125,7 +13159,7 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>503</v>
       </c>
@@ -13160,7 +13194,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="6" t="s">
         <v>504</v>
       </c>
@@ -13195,7 +13229,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
         <v>508</v>
       </c>
@@ -13230,7 +13264,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
         <v>505</v>
       </c>
@@ -13265,7 +13299,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="6" t="s">
         <v>509</v>
       </c>
@@ -13300,7 +13334,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
         <v>506</v>
       </c>
@@ -13335,7 +13369,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="6" t="s">
         <v>510</v>
       </c>
@@ -13370,7 +13404,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
         <v>507</v>
       </c>
@@ -13405,7 +13439,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
         <v>511</v>
       </c>
@@ -13440,7 +13474,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
         <v>512</v>
       </c>
@@ -13475,7 +13509,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="4" t="s">
         <v>513</v>
       </c>
@@ -13510,7 +13544,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="6" t="s">
         <v>514</v>
       </c>
@@ -13545,7 +13579,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="6" t="s">
         <v>515</v>
       </c>
@@ -13580,7 +13614,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
         <v>516</v>
       </c>
@@ -13615,7 +13649,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
         <v>517</v>
       </c>
@@ -13650,7 +13684,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="6" t="s">
         <v>518</v>
       </c>
@@ -13685,7 +13719,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
         <v>519</v>
       </c>
@@ -13720,7 +13754,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="6" t="s">
         <v>520</v>
       </c>
@@ -13754,7 +13788,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
         <v>521</v>
       </c>
@@ -13789,7 +13823,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" s="6" t="s">
         <v>498</v>
       </c>
@@ -13818,7 +13852,7 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>522</v>
       </c>
@@ -13853,7 +13887,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
         <v>523</v>
       </c>
@@ -13888,7 +13922,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
         <v>525</v>
       </c>
@@ -13923,7 +13957,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="6" t="s">
         <v>497</v>
       </c>
@@ -13952,7 +13986,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="4" t="s">
         <v>524</v>
       </c>
@@ -13987,11 +14021,11 @@
         <v>486</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="6"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K31">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K31">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13999,263 +14033,261 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.19921875" customWidth="1"/>
+    <col min="2" max="2" width="18.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="14.55" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
-        <v>496</v>
+        <v>500</v>
       </c>
       <c r="B1" t="s">
         <v>526</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
-        <v>500</v>
+        <v>552</v>
       </c>
       <c r="B2" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>499</v>
+      </c>
+      <c r="B3" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="B4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="B5" t="s">
         <v>528</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
-        <v>502</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="B6" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="B7" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="14.55" x14ac:dyDescent="0.4">
-      <c r="A6" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="B8" t="s">
         <v>531</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="B9" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>508</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="B10" t="s">
         <v>533</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="B11" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="6" t="s">
-        <v>509</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>507</v>
+      </c>
+      <c r="B12" t="s">
         <v>535</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="14.55" x14ac:dyDescent="0.4">
-      <c r="A11" s="4" t="s">
-        <v>506</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>511</v>
+      </c>
+      <c r="B13" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="6" t="s">
-        <v>510</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="B14" t="s">
         <v>537</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>507</v>
-      </c>
-      <c r="B13" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>513</v>
+      </c>
+      <c r="B15" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="B14" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="B16" t="s">
         <v>539</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>512</v>
-      </c>
-      <c r="B15" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A17" s="6" t="s">
+        <v>515</v>
+      </c>
+      <c r="B17" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>513</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A18" s="6" t="s">
+        <v>516</v>
+      </c>
+      <c r="B18" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="B17" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>517</v>
+      </c>
+      <c r="B19" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A20" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="B20" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A21" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="B21" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.55" x14ac:dyDescent="0.4">
-      <c r="A20" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="B20" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A22" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="B22" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="B21" t="s">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="6" t="s">
-        <v>519</v>
-      </c>
-      <c r="B22" t="s">
-        <v>547</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="6" t="s">
-        <v>520</v>
+        <v>558</v>
       </c>
       <c r="B23" t="s">
-        <v>548</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.55" x14ac:dyDescent="0.4">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
         <v>521</v>
       </c>
       <c r="B24" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A25" s="6" t="s">
         <v>498</v>
       </c>
       <c r="B25" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
         <v>522</v>
       </c>
-      <c r="B26" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="10" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
         <v>523</v>
       </c>
       <c r="B27" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>525</v>
+        <v>555</v>
       </c>
       <c r="B28" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A29" s="6" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B29" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
         <v>524</v>
       </c>
       <c r="B30" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A1:B30">
-    <sortCondition ref="A1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>